<commit_message>
Corrected the create_term method, had missed passing a required argement
</commit_message>
<xml_diff>
--- a/Enterprise-Glossary-Terms.xlsx
+++ b/Enterprise-Glossary-Terms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhananjaypunekar/Documents/Landsec-GitHub/Purview-POC-Elastacloud/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhananjaypunekar/Documents/Purview-Glossary-Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493F9E94-DCAD-7B4F-9B4C-817D889D4D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2650D9-750E-2E40-B4A2-87358564AD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B8115C91-8359-1F45-8E80-4C2D480DD7CD}"/>
+    <workbookView xWindow="-11500" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{B8115C91-8359-1F45-8E80-4C2D480DD7CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,14 +553,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F312C43-2ABB-7547-B2F6-AE6D19A6A301}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E22" sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>